<commit_message>
OMS-52, OMS-53 testcases added
</commit_message>
<xml_diff>
--- a/TestData/Inventory_Testdata.xlsx
+++ b/TestData/Inventory_Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B199DF72-FCB2-488F-B42A-8BC0EFA00B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAACC8D6-7746-4131-A41D-5530DE89C474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="540" windowWidth="15375" windowHeight="7875" xr2:uid="{6D745D7C-0653-42F1-A280-8DCEAF7F6AA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D745D7C-0653-42F1-A280-8DCEAF7F6AA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory_data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -44,9 +44,6 @@
     <t>SKU</t>
   </si>
   <si>
-    <t>MFNpartNumber</t>
-  </si>
-  <si>
     <t>VendorBusinessManager</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>CHRIS RICHARDSON</t>
   </si>
   <si>
-    <t>VMA751S9FI1AL0</t>
-  </si>
-  <si>
     <t>CISCO SYSTEMS AUST.</t>
   </si>
   <si>
@@ -69,6 +63,15 @@
   </si>
   <si>
     <t>AU</t>
+  </si>
+  <si>
+    <t>0005467074</t>
+  </si>
+  <si>
+    <t>MFNPartNumber</t>
+  </si>
+  <si>
+    <t>AA.00.0012.17</t>
   </si>
 </sst>
 </file>
@@ -118,13 +121,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,16 +450,16 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -464,33 +470,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OMS-57, OMS-54 testcase added
</commit_message>
<xml_diff>
--- a/TestData/Inventory_Testdata.xlsx
+++ b/TestData/Inventory_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAACC8D6-7746-4131-A41D-5530DE89C474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DAA855-F13D-4458-B3D0-449A016F0A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D745D7C-0653-42F1-A280-8DCEAF7F6AA8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -72,6 +72,18 @@
   </si>
   <si>
     <t>AA.00.0012.17</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>CM - Cost Structure</t>
+  </si>
+  <si>
+    <t>cost structure</t>
+  </si>
+  <si>
+    <t>Actions</t>
   </si>
 </sst>
 </file>
@@ -447,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8515E64-B5AC-47AD-A6CE-4F4F8257F403}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +474,7 @@
     <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,8 +493,14 @@
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -500,6 +518,12 @@
       </c>
       <c r="F2" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OMS-60, OMS-61 testcase added
</commit_message>
<xml_diff>
--- a/TestData/Inventory_Testdata.xlsx
+++ b/TestData/Inventory_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DAA855-F13D-4458-B3D0-449A016F0A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0A01E9-2919-4C06-82E2-F3FCA287D05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D745D7C-0653-42F1-A280-8DCEAF7F6AA8}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>FeatureFileName</t>
   </si>
   <si>
-    <t>SKU</t>
-  </si>
-  <si>
     <t>VendorBusinessManager</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>0005467074</t>
   </si>
   <si>
-    <t>MFNPartNumber</t>
-  </si>
-  <si>
     <t>AA.00.0012.17</t>
   </si>
   <si>
@@ -80,17 +74,47 @@
     <t>CM - Cost Structure</t>
   </si>
   <si>
-    <t>cost structure</t>
-  </si>
-  <si>
     <t>Actions</t>
+  </si>
+  <si>
+    <t>AgingSKU</t>
+  </si>
+  <si>
+    <t>AgingMFNPartNumber</t>
+  </si>
+  <si>
+    <t>0005352280</t>
+  </si>
+  <si>
+    <t>DOCK182AUZ</t>
+  </si>
+  <si>
+    <t>CM - Pricing</t>
+  </si>
+  <si>
+    <t>test cost structure</t>
+  </si>
+  <si>
+    <t>test pricing</t>
+  </si>
+  <si>
+    <t>UnderperformingSKU</t>
+  </si>
+  <si>
+    <t>UnderperformingMFNPartNumber</t>
+  </si>
+  <si>
+    <t>UpdateAction</t>
+  </si>
+  <si>
+    <t>UpdateComment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +135,13 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -145,6 +176,8 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8515E64-B5AC-47AD-A6CE-4F4F8257F403}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,58 +505,86 @@
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
+      <c r="J2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 100 aging testcases added
</commit_message>
<xml_diff>
--- a/TestData/Inventory_Testdata.xlsx
+++ b/TestData/Inventory_Testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0A01E9-2919-4C06-82E2-F3FCA287D05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E967371D-3CA7-432B-BEE3-282EBA4188A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D745D7C-0653-42F1-A280-8DCEAF7F6AA8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -83,38 +83,56 @@
     <t>AgingMFNPartNumber</t>
   </si>
   <si>
+    <t>DOCK182AUZ</t>
+  </si>
+  <si>
+    <t>CM - Pricing</t>
+  </si>
+  <si>
+    <t>test cost structure</t>
+  </si>
+  <si>
+    <t>UnderperformingSKU</t>
+  </si>
+  <si>
+    <t>UnderperformingMFNPartNumber</t>
+  </si>
+  <si>
+    <t>DIO - RMA</t>
+  </si>
+  <si>
+    <t>rma test</t>
+  </si>
+  <si>
     <t>0005352280</t>
   </si>
   <si>
-    <t>DOCK182AUZ</t>
-  </si>
-  <si>
-    <t>CM - Pricing</t>
-  </si>
-  <si>
-    <t>test cost structure</t>
-  </si>
-  <si>
-    <t>test pricing</t>
-  </si>
-  <si>
-    <t>UnderperformingSKU</t>
-  </si>
-  <si>
-    <t>UnderperformingMFNPartNumber</t>
-  </si>
-  <si>
-    <t>UpdateAction</t>
-  </si>
-  <si>
-    <t>UpdateComment</t>
+    <t>9YG957</t>
+  </si>
+  <si>
+    <t>ROBERT BROWN</t>
+  </si>
+  <si>
+    <t>JUNIPER</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MLYU3AM/A</t>
+  </si>
+  <si>
+    <t>iinventory_management_action_planning</t>
+  </si>
+  <si>
+    <t>pricing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +161,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -178,6 +201,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8515E64-B5AC-47AD-A6CE-4F4F8257F403}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,10 +539,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -541,12 +565,8 @@
       <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -569,22 +589,60 @@
         <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
+      <c r="H4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 100 Aging sku testcases added
</commit_message>
<xml_diff>
--- a/TestData/Inventory_Testdata.xlsx
+++ b/TestData/Inventory_Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E967371D-3CA7-432B-BEE3-282EBA4188A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8D7347-E92E-42CB-A590-F2B98EB4491F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D745D7C-0653-42F1-A280-8DCEAF7F6AA8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>CM - Cost Structure</t>
-  </si>
-  <si>
     <t>Actions</t>
   </si>
   <si>
@@ -86,12 +83,6 @@
     <t>DOCK182AUZ</t>
   </si>
   <si>
-    <t>CM - Pricing</t>
-  </si>
-  <si>
-    <t>test cost structure</t>
-  </si>
-  <si>
     <t>UnderperformingSKU</t>
   </si>
   <si>
@@ -105,27 +96,6 @@
   </si>
   <si>
     <t>0005352280</t>
-  </si>
-  <si>
-    <t>9YG957</t>
-  </si>
-  <si>
-    <t>ROBERT BROWN</t>
-  </si>
-  <si>
-    <t>JUNIPER</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>MLYU3AM/A</t>
-  </si>
-  <si>
-    <t>iinventory_management_action_planning</t>
-  </si>
-  <si>
-    <t>pricing</t>
   </si>
 </sst>
 </file>
@@ -518,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8515E64-B5AC-47AD-A6CE-4F4F8257F403}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,10 +509,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -554,16 +524,16 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -589,61 +559,36 @@
         <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="C6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="G6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>